<commit_message>
Code: Faltan los SVN
</commit_message>
<xml_diff>
--- a/bdd/bdd.xlsx
+++ b/bdd/bdd.xlsx
@@ -8,24 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abraham\Documents\Machine-Learning-con-Jupiter\bdd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E037DF36-5C28-4FD5-8A16-9C490F8AA00C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{011D721F-946A-41C0-90B1-5ACF4F290558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21135" yWindow="3960" windowWidth="14085" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22635" yWindow="2055" windowWidth="14085" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="55">
   <si>
     <t>Code</t>
   </si>
@@ -209,6 +219,9 @@
   </si>
   <si>
     <t>TENS</t>
+  </si>
+  <si>
+    <t>NPROGNOSIS</t>
   </si>
 </sst>
 </file>
@@ -731,15 +744,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AP47"/>
+  <dimension ref="A1:AQ47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="AL1" sqref="AL1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:42" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -866,8 +879,11 @@
       <c r="AP1" t="s">
         <v>41</v>
       </c>
+      <c r="AQ1" s="9" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="2" spans="1:42" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -991,8 +1007,12 @@
       <c r="AO2" s="18">
         <v>18.586835371280198</v>
       </c>
+      <c r="AQ2">
+        <f>IF(AL2="Bad",2,IF(AL2="Good",1,3))</f>
+        <v>2</v>
+      </c>
     </row>
-    <row r="3" spans="1:42" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1116,8 +1136,12 @@
       <c r="AO3" s="19">
         <v>1.2634414824451099</v>
       </c>
+      <c r="AQ3">
+        <f t="shared" ref="AQ3:AQ46" si="0">IF(AL3="Bad",2,IF(AL3="Good",1,3))</f>
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:42" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1244,8 +1268,12 @@
       <c r="AP4">
         <v>33375000000</v>
       </c>
+      <c r="AQ4">
+        <f>IF(AL4="Bad",2,IF(AL4="Good",1,3))</f>
+        <v>3</v>
+      </c>
     </row>
-    <row r="5" spans="1:42" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1369,8 +1397,12 @@
       <c r="AO5" s="21">
         <v>96.544126203520193</v>
       </c>
+      <c r="AQ5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:42" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1497,8 +1529,12 @@
       <c r="AP6">
         <v>13499000000</v>
       </c>
+      <c r="AQ6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="7" spans="1:42" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1625,8 +1661,12 @@
       <c r="AP7">
         <v>17812500000</v>
       </c>
+      <c r="AQ7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="8" spans="1:42" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
@@ -1750,8 +1790,12 @@
       <c r="AO8" s="23">
         <v>13.519903797866199</v>
       </c>
+      <c r="AQ8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="9" spans="1:42" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>11</v>
       </c>
@@ -1878,8 +1922,12 @@
       <c r="AP9">
         <v>21425000000</v>
       </c>
+      <c r="AQ9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:42" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>12</v>
       </c>
@@ -2006,8 +2054,12 @@
       <c r="AP10">
         <v>12500000000</v>
       </c>
+      <c r="AQ10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="11" spans="1:42" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>14</v>
       </c>
@@ -2134,8 +2186,12 @@
       <c r="AP11">
         <v>23312500000</v>
       </c>
+      <c r="AQ11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="12" spans="1:42" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>16</v>
       </c>
@@ -2262,8 +2318,12 @@
       <c r="AP12">
         <v>36875000000</v>
       </c>
+      <c r="AQ12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="13" spans="1:42" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>18</v>
       </c>
@@ -2390,8 +2450,12 @@
       <c r="AP13">
         <v>19050000000</v>
       </c>
+      <c r="AQ13">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="14" spans="1:42" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>19</v>
       </c>
@@ -2515,8 +2579,12 @@
       <c r="AO14" s="21">
         <v>35.534072508723703</v>
       </c>
+      <c r="AQ14">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="15" spans="1:42" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>23</v>
       </c>
@@ -2643,8 +2711,12 @@
       <c r="AP15">
         <v>21125000000</v>
       </c>
+      <c r="AQ15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="16" spans="1:42" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>24</v>
       </c>
@@ -2771,8 +2843,12 @@
       <c r="AP16">
         <v>8937500500</v>
       </c>
+      <c r="AQ16">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="17" spans="1:42" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>25</v>
       </c>
@@ -2896,8 +2972,12 @@
       <c r="AO17" s="23">
         <v>4.1632354056519896</v>
       </c>
+      <c r="AQ17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="18" spans="1:42" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>27</v>
       </c>
@@ -3021,8 +3101,12 @@
       <c r="AO18" s="21">
         <v>14.3998709020295</v>
       </c>
+      <c r="AQ18">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="19" spans="1:42" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>29</v>
       </c>
@@ -3149,8 +3233,12 @@
       <c r="AP19">
         <v>6262500000</v>
       </c>
+      <c r="AQ19">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="20" spans="1:42" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>30</v>
       </c>
@@ -3277,8 +3365,12 @@
       <c r="AP20">
         <v>22725000000</v>
       </c>
+      <c r="AQ20">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="21" spans="1:42" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>31</v>
       </c>
@@ -3405,8 +3497,12 @@
       <c r="AP21">
         <v>25087500000</v>
       </c>
+      <c r="AQ21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="22" spans="1:42" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:43" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="25">
         <v>32</v>
       </c>
@@ -3533,8 +3629,12 @@
       <c r="AP22">
         <v>6925000000</v>
       </c>
+      <c r="AQ22">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
     </row>
-    <row r="23" spans="1:42" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:43" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>34</v>
       </c>
@@ -3658,8 +3758,12 @@
       <c r="AO23" s="18">
         <v>34.1384176856401</v>
       </c>
+      <c r="AQ23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="24" spans="1:42" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>36</v>
       </c>
@@ -3783,8 +3887,12 @@
       <c r="AO24" s="23">
         <v>63.357695358048403</v>
       </c>
+      <c r="AQ24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="25" spans="1:42" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>37</v>
       </c>
@@ -3908,8 +4016,12 @@
       <c r="AO25" s="23">
         <v>41.744564650413203</v>
       </c>
+      <c r="AQ25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="26" spans="1:42" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>39</v>
       </c>
@@ -4033,8 +4145,12 @@
       <c r="AO26" s="19">
         <v>2.8099982414887799</v>
       </c>
+      <c r="AQ26">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="27" spans="1:42" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>40</v>
       </c>
@@ -4161,8 +4277,12 @@
       <c r="AP27">
         <v>407000000</v>
       </c>
+      <c r="AQ27">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="28" spans="1:42" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>44</v>
       </c>
@@ -4286,8 +4406,12 @@
       <c r="AO28" s="23">
         <v>71.709101856884303</v>
       </c>
+      <c r="AQ28">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="29" spans="1:42" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>45</v>
       </c>
@@ -4411,8 +4535,12 @@
       <c r="AO29" s="32">
         <v>58.462687459382501</v>
       </c>
+      <c r="AQ29">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="30" spans="1:42" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:43" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>49</v>
       </c>
@@ -4536,8 +4664,12 @@
       <c r="AO30" s="19">
         <v>15.9943946123361</v>
       </c>
+      <c r="AQ30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="31" spans="1:42" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:43" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>51</v>
       </c>
@@ -4661,8 +4793,12 @@
       <c r="AO31" s="18">
         <v>18.985593892161202</v>
       </c>
+      <c r="AQ31">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="32" spans="1:42" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>52</v>
       </c>
@@ -4786,8 +4922,12 @@
       <c r="AO32" s="23">
         <v>0.52882702189936903</v>
       </c>
+      <c r="AQ32">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="33" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>57</v>
       </c>
@@ -4911,8 +5051,12 @@
       <c r="AO33" s="18">
         <v>48.693103697797397</v>
       </c>
+      <c r="AQ33">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="34" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>58</v>
       </c>
@@ -5036,8 +5180,12 @@
       <c r="AO34" s="18">
         <v>1.8389774942772501</v>
       </c>
+      <c r="AQ34">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="35" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>59</v>
       </c>
@@ -5161,8 +5309,12 @@
       <c r="AO35" s="23">
         <v>1.4954249963016599</v>
       </c>
+      <c r="AQ35">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="36" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>61</v>
       </c>
@@ -5286,8 +5438,12 @@
       <c r="AO36" s="18">
         <v>54.873860771453302</v>
       </c>
+      <c r="AQ36">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="37" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>63</v>
       </c>
@@ -5411,8 +5567,12 @@
       <c r="AO37" s="23">
         <v>10.658773793635399</v>
       </c>
+      <c r="AQ37">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="38" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:43" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>64</v>
       </c>
@@ -5536,8 +5696,12 @@
       <c r="AO38" s="18">
         <v>42.113588103260597</v>
       </c>
+      <c r="AQ38">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="39" spans="1:41" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:43" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>66</v>
       </c>
@@ -5661,8 +5825,12 @@
       <c r="AO39" s="18">
         <v>77.603096461671598</v>
       </c>
+      <c r="AQ39">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="40" spans="1:41" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:43" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>67</v>
       </c>
@@ -5786,8 +5954,12 @@
       <c r="AO40" s="19">
         <v>0.45149918394718502</v>
       </c>
+      <c r="AQ40">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
     </row>
-    <row r="41" spans="1:41" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:43" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>68</v>
       </c>
@@ -5911,8 +6083,12 @@
       <c r="AO41" s="18">
         <v>41.316071061498498</v>
       </c>
+      <c r="AQ41">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="42" spans="1:41" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:43" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>71</v>
       </c>
@@ -6036,8 +6212,12 @@
       <c r="AO42" s="21">
         <v>24.966971705376601</v>
       </c>
+      <c r="AQ42">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="43" spans="1:41" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:43" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>72</v>
       </c>
@@ -6161,8 +6341,12 @@
       <c r="AO43" s="18">
         <v>18.7862146317207</v>
       </c>
+      <c r="AQ43">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="44" spans="1:41" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:43" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>75</v>
       </c>
@@ -6286,8 +6470,12 @@
       <c r="AO44" s="23">
         <v>15.7237471795034</v>
       </c>
+      <c r="AQ44">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="45" spans="1:41" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:43" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>76</v>
       </c>
@@ -6411,8 +6599,12 @@
       <c r="AO45" s="18">
         <v>15.7955257251131</v>
       </c>
+      <c r="AQ45">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="46" spans="1:41" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:43" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="35" t="s">
         <v>53</v>
       </c>
@@ -6536,8 +6728,12 @@
       <c r="AO46" s="31">
         <v>77.204337940790595</v>
       </c>
+      <c r="AQ46">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
     </row>
-    <row r="47" spans="1:41" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:43" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="E2:AO46">
     <cfRule type="containsBlanks" dxfId="0" priority="1">

</xml_diff>